<commit_message>
update test spreadsheet for consistency
</commit_message>
<xml_diff>
--- a/input_spreadsheets/InputForCode_tests.xlsx
+++ b/input_spreadsheets/InputForCode_tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" tabRatio="500" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="82">
   <si>
     <t>indicators</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>fraction poor</t>
+  </si>
+  <si>
+    <t>fraction food insecure (not poor)</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -548,6 +551,9 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,6 +586,57 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="1025" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -881,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -941,6 +998,14 @@
       </c>
       <c r="B6">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="33">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -1716,7 +1781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>42</v>
       </c>
@@ -2165,7 +2230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -3129,7 +3194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>500</v>
       </c>
@@ -3845,7 +3910,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>